<commit_message>
remove print, remove -asg from name wen ru code
</commit_message>
<xml_diff>
--- a/dataset/engine-asg/cpu.xlsx
+++ b/dataset/engine-asg/cpu.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,7 +438,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>05/26/2021 01:05:30</t>
+          <t>05/26/2021 01:55:32</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -448,221 +448,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>05/26/2021 01:06:31</t>
+          <t>05/26/2021 01:56:34</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>0.3333</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:07:33</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.3333</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:08:35</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.3333</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:09:37</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.3390000000000001</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:10:40</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.3333</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:11:42</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.3279</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:12:44</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:13:46</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:14:49</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0.3306</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:15:52</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0.3362</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:16:55</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0.3362</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:17:58</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>36.1667</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:19:01</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>49.1667</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:20:05</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>37.7966</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:21:09</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:26:21</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>36.6102</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:27:24</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>26.806</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:28:27</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>18.66395</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:33:39</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>29.7326</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:34:43</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>11.11023333333333</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:35:47</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>15.85636666666667</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>05/26/2021 01:41:07</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>0.331275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>